<commit_message>
Fix: removed dotenv and updated app.py for Streamlit Cloud
</commit_message>
<xml_diff>
--- a/pune_doctors_streamlit.xlsx
+++ b/pune_doctors_streamlit.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,749 +493,3522 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Dr. Mustapure's Child Clinic</t>
+          <t>Oliva Skin, Hair &amp; Laser Clinic Aundh, Pune | Best Dermatologist In Pune For Skin Rejuvenation &amp; Hair Loss Treatments</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Pediatrician</t>
+          <t>Dermatologist</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Dr. Mustapure's Child Clinic</t>
+          <t>Oliva Skin, Hair &amp; Laser Clinic Aundh, Pune | Best Dermatologist In Pune For Skin Rejuvenation &amp; Hair Loss Treatments</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2nd floor, Grand Heritage, Kaspate Wasti Rd, opposite Ambience hotel, Vishnu Dev Nagar, Wakad, Pimpri-Chinchwad, Maharashtra 411057, India</t>
+          <t>Ground Floor, Jai Hind Building, Khond Arcade, Parihar chowk, ITT Road, opposite State Bank Of India, Sanghvi Nagar, Aundh, Pune, Maharashtra 411067, India</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>+91 70831 40369</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
+          <t>+91 88862 77700</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>https://www.olivaclinic.com/pune/skin-hair-clinic-in-aundh/?utm_source=BL&amp;utm_medium=Website&amp;utm_campaign=Aundh</t>
+        </is>
+      </c>
       <c r="G2" t="n">
         <v>4.9</v>
       </c>
       <c r="H2" t="n">
-        <v>386</v>
+        <v>344</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>We’ve been consulting this doctor for quite some time now for both of our daughters, and the experience has always been exceptional. He’s ex | Highly Recommended Pediatrician 👌⭐👼 I have been consulting Dr. Mustapure sir for my son for almost two years now, and the support we’ve rece | We are having good experience of doctor's treatment for my kid. He is our regular doctor for my kid. My son is getting treated in Mustapure' | I have been consulting Dr. Mustapure for my child for the past 3 years, and I can confidently say he is one of the most intelligent and comp | THE PRECISE PEDIATRIC CARE YOUR CHILD NEEDS 😊  Our newborn baby visited Dr. Mustapure for her very first routine visit. Since then she is in</t>
+          <t>—</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>ChIJrU0gQe-7wjsRXDfgDEtaBIs</t>
+          <t>ChIJm4JBROe_wjsRATsEunHCDJY</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Wakad, Pune</t>
+          <t>Aundh, Pune</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Dr.Kapil Jadhav</t>
+          <t>Avanti Skin Clinic</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Pediatrician</t>
+          <t>Dermatologist</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Dr.Kapil Jadhav</t>
+          <t>Avanti Skin Clinic</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Clinic No.1/2, Dr. Mande's Clinic, VARDHAMAN PLAZA, opp. Dynasty Society Road, near Radha Pure Veg, Kaspate Wasti, Wakad, Pune, Pimpri-Chinchwad, Maharashtra 411057, India</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
+          <t>Shop No - 5, Stellar Enclave, opp. WESTEND MALL, Ward No. 8, Aundh Gaon, Aundh, Pune, Maharashtra 411067, India</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>+91 80108 40653</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>https://www.avantiskinclinic.com/</t>
+        </is>
+      </c>
       <c r="G3" t="n">
-        <v>4.6</v>
+        <v>4.8</v>
       </c>
       <c r="H3" t="n">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>When we contacted the doctor, he said he would arrive in 10–15 minutes. However, even after waiting over 40 + minutes at the clinic, the rec | The best doctor I got for my son..He is very knowledgeable, kind and listens to your queries..always supported us and attended us whenever t | Worst experience of my life, lacks expertise, rude , money minded, have to visit another doctor everytime we visited him, does not check pat | I've have visited Dr. Kapil's clinic 3-4 times, and I've always been impressed with the minimal wait time - never more than 10-15 minutes! A | Doctor gave vaccination and the child is in pain. He just gave the injection as if the child is some animal. He overcharged. Not recommended</t>
+          <t>—</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>ChIJtSsVsRO5wjsRvFpxurCZT60</t>
+          <t>ChIJAUEL5G-_wjsRZsq5cKa0NWo</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Wakad, Pune</t>
+          <t>Aundh, Pune</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Dr. Nikhil Patil - Pediatrician, Child Clinic, Child Doctor, Child Specialist in Hinjewadi, Pediatrician in Wakad</t>
+          <t>Esthetiq Curve by Dr. Juhi Talreja Skin Hair Laser Clinic Aundh</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Pediatrician</t>
+          <t>Dermatologist</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Dr. Nikhil Patil - Pediatrician, Child Clinic, Child Doctor, Child Specialist in Hinjewadi, Pediatrician in Wakad</t>
+          <t>Esthetiq Curve by Dr. Juhi Talreja Skin Hair Laser Clinic Aundh</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2nd Floor, Swasti Clinic, Ram Height, near D' Mart, above Bata Showroom, Hinjawadi, Pune, Pimpri-Chinchwad, Maharashtra 411057, India</t>
+          <t>Office No 103, 1st floor, Astral Court, Petrol Pump, opposite Ramchandra Ganpatrao Gaikwad Road, near Reliance fresh, Marutirao Gaikwad Nagar, Aundh, Pune, Maharashtra 411007, India</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>+91 72492 98207</t>
+          <t>+91 98348 52142</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://swasticlinicpune.in/</t>
+          <t>https://www.drjuhitalreja.com/</t>
         </is>
       </c>
       <c r="G4" t="n">
         <v>4.9</v>
       </c>
       <c r="H4" t="n">
-        <v>234</v>
+        <v>155</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t xml:space="preserve">We’ve had a truly wonderful experience with Dr. Nikhil Patil, and I feel compelled to share it for other parents who are looking for a trust | I had visited the clinic after hearing a lot of positive feedback from the family members of the patients. I am really glad and happy to hav | Dr. Nikhil Patil is an excellent doctor. We consulted him for our daughter when she was suffering from high fever. We were extremely worried | As first-time parents, entrusting our newborn's care to Dr. Nikhil Patil is been and an on going extraordinary experience.  When I visited D | As first-time parents, entrusting our newborn's care to Dr. Nikhil Patil at Lifetree Hospital in Hinjewadi, Pune, has been an extraordinary </t>
+          <t>—</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>ChIJUZwykXq7wjsRlJZEPoLlGmA</t>
+          <t>ChIJZRL7Vdq5wjsRges3_Kcxbvs</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Wakad, Pune</t>
+          <t>Aundh, Pune</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Dr. Yogesh Jadhav</t>
+          <t>PURE SKIN &amp; HAIR TRANSPLANT CLINIC PUNE</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Pediatrician</t>
+          <t>Dermatologist</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Dr. Yogesh Jadhav</t>
+          <t>PURE SKIN &amp; HAIR TRANSPLANT CLINIC PUNE</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>201, Cubes Commercial Complex, Datta Mandir Rd, above Apricot Hotel, Shankar Kalat Nagar, Wakad, Pune, Pimpri-Chinchwad, Maharashtra 411057, India</t>
+          <t>First Floor,Hrishikesh Dham, Parihar chowk, above Parihar and Ramesh store, opposite wellness forever, Sanghvi Nagar, Aundh, Pune, Maharashtra 411067, India</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>+91 98908 30804</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr"/>
+          <t>+91 95183 80486</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>https://pureskinclinicpune.com/</t>
+        </is>
+      </c>
       <c r="G5" t="n">
         <v>4.8</v>
       </c>
       <c r="H5" t="n">
-        <v>101</v>
+        <v>286</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t xml:space="preserve">I had a wonderful experience at Tender Care Baby Hospital, and I want to extend a special thank you to Pediatrician Dr. Yogesh Jadhav. His e | Dr Yogesh is just awesome. He is very friendly with kids. He is very patient and helps to put all parent’s anxieties to rest. Most important | He is THE BEST DOCTOR for my kids. He is always there whenever I needed him for any case whether it is a casual or emergency situation. If n | We had an exceptional experience with Dr. Yogesh Jadhav as our pediatrician.  Dr. Jadhav took the time to explain the dietary needs of our c | Dr. Yogesh is the best pediatric doctor I ever seen. I regular visit his clinic if my child has  any problem.  He is  very cool and results </t>
+          <t>—</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>ChIJsYVv8Qm5wjsRwq28tCCCUlc</t>
+          <t>ChIJU5zMT2S_wjsRgsXHMLe9mS8</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Wakad, Pune</t>
+          <t>Aundh, Pune</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Dr. Swapnil Janbandhu - Curesta Speciality Clinic</t>
+          <t>Kaya Clinic - Aundh, Pune: Laser Hair Reduction, Acne Scar, Hair Loss, Skin Lightening &amp; Fat Loss Treatments</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Pediatrician</t>
+          <t>Dermatologist</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Dr. Swapnil Janbandhu - Curesta Speciality Clinic</t>
+          <t>Kaya Clinic - Aundh, Pune: Laser Hair Reduction, Acne Scar, Hair Loss, Skin Lightening &amp; Fat Loss Treatments</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Office no. 204 and 205, Oriana Crest commercial complex, Datta Mandir Rd, Postal Colony, Shankar Kalat Nagar, Wakad, Pune, Pimpri-Chinchwad, Maharashtra 411057, India</t>
+          <t>Ground Floor, Daya Prabha House, ITI Rd, opposite KRA Jewellers, Ward No. 8, Pushpak Park, Aundh, Pune, Maharashtra 411007, India</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>+91 98234 46644</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
+          <t>+91 86575 69413</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>https://clinics.kaya.in/kaya-clinic/pune/Aundh/kaya-clinic-aundh-pune-in-Aundh-pune--5K7ct7/home</t>
+        </is>
+      </c>
       <c r="G6" t="n">
-        <v>4.8</v>
+        <v>4.7</v>
       </c>
       <c r="H6" t="n">
-        <v>87</v>
+        <v>775</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>We had been visiting doc Swapnil Janbandhu since last 7 years for our kids . He is very patient and provides ample time for all  queries and | Dr. Swapnil is an excellent physician. Very caring and personable. The office staff is top notch. We couldn't have asked for a better Paedia | We had a very bad experience recently with Dr. Swapnil Janbandhu. We did OPD consultation for our child who had severe cough, headache and h | Dr Swapnil is truly awesome.  He is kind,caring ,patient incredibly knowledgeable and a real magician with babies. He is well read , has a w | Dr. Swapnil Janbandhu is one of the best pediatrician in PCMC Area. His way of treatment and diagnosis is really commendable. He is very kno</t>
+          <t>—</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>ChIJO5h5q8u5wjsR_xpSncpWEyQ</t>
+          <t>ChIJ13uYfzu_wjsRp3izC1s_e7s</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Wakad, Pune</t>
+          <t>Aundh, Pune</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Dr Gavhane children ,women clinic Dr Pradip Gavhane best paeditrician ,child specialist,gynacologist Hinjewadi ,Wakad,pune</t>
+          <t>Dr.Ravi Kothari</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Pediatrician</t>
+          <t>Dermatologist</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Dr Gavhane children ,women clinic Dr Pradip Gavhane best paeditrician ,child specialist,gynacologist Hinjewadi ,Wakad,pune</t>
+          <t>Dr.Ravi Kothari</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>shop no 3, Shivkrupa Complex, opposite to D mart, Hinjawadi, Pune, Pimpri-Chinchwad, Maharashtra 411057, India</t>
+          <t>First floor, DP Rd, above Federal Bank, Raagdari Society, Aundh, Pune, Maharashtra 411067, India</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>+91 72767 20084</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr"/>
+          <t>+91 94221 82005</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>https://www.drravikothari.com/</t>
+        </is>
+      </c>
       <c r="G7" t="n">
-        <v>5</v>
+        <v>4.3</v>
       </c>
       <c r="H7" t="n">
-        <v>250</v>
+        <v>159</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Dr Pradip Gavhane is very good Pediatrician in hinjewadi area.My child turn 2 year taking vaccine from 3.5 month &amp; also treatment when he is | Dr Gavhane children,women clinic Hinjewadi is  an excellent center for maternal and child care. The facilities are modern, and the environme | Dr Pradeep Gavhane sir is highly educated and provide the best treatment for child &amp; also give me good guidance about nutrition and food tha | Very good clinic for Gynacological problem's in Hinjewadi area.Dr Pranjali Gavhane treated me with minimum medicines &amp;also gave me good guid | I have been taking my kids to Dr. Pradip Gavhane for a year time,  Dr. Sir gives adequate time, examines properly, records thing properly in</t>
+          <t>—</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>ChIJ_X_ukrK7wjsRNnr_DPOOZl8</t>
+          <t>ChIJAbinFVS_wjsR9R-gw70uRpQ</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Wakad, Pune</t>
+          <t>Aundh, Pune</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Dr.Ganesh Shiwarkar ,Sparkle Kids Clinic, wakad</t>
+          <t>Skin &amp; Surgery International &amp; Asia Institute Of Hair Transplant - Dr Rituja Jaju</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Pediatrician</t>
+          <t>Dermatologist</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Dr.Ganesh Shiwarkar ,Sparkle Kids Clinic, wakad</t>
+          <t>Skin &amp; Surgery International &amp; Asia Institute Of Hair Transplant - Dr Rituja Jaju</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Shree Ganesh Imperia Square, shop no.105,1st floor,S no. 175/3, opp. Omega paradise soc, behind postal colony, Shankar Kalat Nagar, Wakad, Pune, Pimpri-Chinchwad, Maharashtra 411057, India</t>
+          <t>1st Floor, Raviraj Appartment, Parihar Chowk, DP Rd, above Parihar Departmental Store and Neeta Volvo, Aundh, Pune, Maharashtra 411067, India</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>+91 98902 58281</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
+          <t>+91 90966 94007</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>https://www.skinhairsurgery.com/</t>
+        </is>
+      </c>
       <c r="G8" t="n">
-        <v>4.8</v>
+        <v>4.7</v>
       </c>
       <c r="H8" t="n">
-        <v>165</v>
+        <v>461</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>The accessibility to Dr. Ganesh Shivarkar is worth a million bucks! We have never had any issues getting our baby in when they need to see h | Dr Ganesh Shiwarkar  is the best Pediatrician doctor in pune. He is having excellent knowledge with so many years of Experience, very helpfu | Dr. Ganesh shiwarkar is always accessible. His consultation is very good. He is calm &amp; composed. We have very good experience at his clinic. | It always great to visit Dr. Ganesh. He never fails to respond to my emergency message. Being a new mom I get panicked about everything rela | Dr.Ganesh is an exceptional pediatrician,Our child has been under their care for almost 9 years,We have always been impressed with his kindn</t>
+          <t>—</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>ChIJLx1oJ2u5wjsRUwySJnGWDGY</t>
+          <t>ChIJ-RIaDDC_wjsRu5TJIvalztY</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Wakad, Pune</t>
+          <t>Aundh, Pune</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Dr. Munde's Child &amp; Vaccination Clinic</t>
+          <t>Dr Anuradha Patil Dermatologist in Aundh, Sanghvi, Pune</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Pediatrician</t>
+          <t>Dermatologist</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Dr. Munde's Child &amp; Vaccination Clinic</t>
+          <t>Dr Anuradha Patil Dermatologist in Aundh, Sanghvi, Pune</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Shop no. 1B, WINDWARDS SOCIETY, E - Wing, Chatrapati Chowk Rd, Kaspate Wasti, Wakad, Pimpri-Chinchwad, Pune, Maharashtra 411057, India</t>
+          <t>Office No 201,2nd Floor, Neo Skin and Hair Clinic, Seasons Rd, above Food Junction, next to Gaikwad Petrol Pump, Marutirao Gaikwad Nagar, Aundh, Pune, Maharashtra 411067, India</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>+91 77096 29988</t>
+          <t>+91 80 4805 5615</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.drmundechildclinic.com/</t>
+          <t>https://www.neoskinhair.com/</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>5</v>
+        <v>4.8</v>
       </c>
       <c r="H9" t="n">
-        <v>121</v>
+        <v>71</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t xml:space="preserve">I recently visited Dr.Munde and had a very positive experience. He is not only highly knowledgeable and experienced, but also incredibly kin | We visited Dr. Munde's clinic for vaccination of my son and had very positive experience. He is very polite explain each and every thing in  | Dr. Tukaram Mundhe is an exceptionally skilled and experienced pediatrician. When my daughter was unwell, we consulted him, and with his acc | Dr Tukaram Munde is truly the best pediatrician we've ever met. They are extremely kind, patient, and knowledgeable. They explain everything | Very good treatment and good nature.  Dr. Tukaram Munde is truly exceptional. Not only did he diagnose my condition accurately, but he also </t>
+          <t>—</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>ChIJOZSbh4y5wjsRn1_nJgvvOSE</t>
+          <t>ChIJcWV4Wme_wjsRD7EU7yb6ItY</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Wakad, Pune</t>
+          <t>Aundh, Pune</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Dr. Avinash Itke - Pediatrician and Neonatologist in Wakad, Pune</t>
+          <t>The Heart Clinic | Dr. Satyajeet Suryawanshi | Heart Specialist | Trusted Cardiac Care in Aundh &amp; Baner</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Pediatrician</t>
+          <t>Cardiologist</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Dr. Avinash Itke - Pediatrician and Neonatologist in Wakad, Pune</t>
+          <t>The Heart Clinic | Dr. Satyajeet Suryawanshi | Heart Specialist | Trusted Cardiac Care in Aundh &amp; Baner</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>S.No. 173, 201, Shankar Kalat Nagar, Thergaon, Datta Mandir Rd, Shankar Kalat Nagar, Wakad, wakad, Pimpri-Chinchwad, Maharashtra 411057, India</t>
+          <t>The Heart Clinic Aundh, Office no 101-102 Astral Court. Near Gaikwad Petrol Pump. Above Reliance fresh Aundh. Aundh Pune: 411007, Marutirao Gaikwad Nagar, Aundh, Pune, Maharashtra 411067, India</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>+91 89285 04499</t>
+          <t>+91 80 4806 6834</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://orionhospital.in/</t>
+          <t>https://www.heartclinicaundh.com/</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>5</v>
+        <v>4.7</v>
       </c>
       <c r="H10" t="n">
-        <v>5</v>
+        <v>175</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>We have been visiting Dr Avinash since the last 2 years for our kids. He has a pleasing temperament, explains everything in detail, is avail | Very humble polite and knowledgeable doctor. I highly recommend others for their kids. | Good experienced.</t>
+          <t>—</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>ChIJtxiA0sS5wjsRN3CrIDUxQyk</t>
+          <t>ChIJq1o9OG2_wjsRBCjV-mgBo0E</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Wakad, Pune</t>
+          <t>Aundh, Pune</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>TINY BLISS CHILD CARE - Dr.Amol Dindgire, Best pediatrician in HINJEWADI, PUNE</t>
+          <t>Dr. Rajdatt Deore</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Pediatrician</t>
+          <t>Cardiologist</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>TINY BLISS CHILD CARE - Dr.Amol Dindgire, Best pediatrician in HINJEWADI, PUNE</t>
+          <t>Dr. Rajdatt Deore</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Sahil plaza, Sai hospital, near bharat petroleum, infront of shatayu hospital, Bhatewara Nagar, Hinjawadi, Pune, Pimpri-Chinchwad, Maharashtra 411057, India</t>
+          <t>Pulse Cardiac-Diabetes Clinic 614, West Avenue, above Atithi Hotel Breman Chawk, Phase 1, Siddarth Nagar Society, Aundh, Pune, Maharashtra 411067, India</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>+91 86696 67846</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr"/>
+          <t>+91 99209 46760</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>http://www.topcardiologistpune.com/</t>
+        </is>
+      </c>
       <c r="G11" t="n">
         <v>4.9</v>
       </c>
       <c r="H11" t="n">
-        <v>391</v>
+        <v>843</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>We had a great experience at Tiny Bliss. Dr. Amol spoke to us very patiently and kindly. He gave us ample time, didn’t rush at all, and genu | He is very nice with kids, and suggests best medication, do not recoomend unneccesaary Reports, also if you go for vaccination he do not cha | Doctor should be personable, great listeners, and empathetic to the concerns of their patients. Mr. Amol have all these qualities. Thanks fo | Dr Amol is very pediatric Dr seen till now. Recently given good treatment for my son for his cough and vomiting treatment. Clear all small d | I highly recommend Dr. Amol as a pediatrician. He is exceptionally knowledgeable and caring, always taking the time to listen to our concern</t>
+          <t>—</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>ChIJyc6ODVm7wjsRj6y_KD0QlmU</t>
+          <t>ChIJ848Gmeq_wjsRWKeTMB2JhGg</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Wakad, Pune</t>
+          <t>Aundh, Pune</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Surya Mother And Child Super Speciality Hospital, Hinjewadi</t>
+          <t>Baner Heart Institute - Dr. Ranjeet Patil - Interventional Cardiologist</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Pediatrician</t>
+          <t>Cardiologist</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Surya Mother And Child Super Speciality Hospital, Hinjewadi</t>
+          <t>Baner Heart Institute - Dr. Ranjeet Patil - Interventional Cardiologist</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Pune Octroi Naka, Sr. No. 8 near Bhujbal Chowk Mumbai Hwy Hinjawadi, Wakad Rd, Bhujbal Vasti, Wakad, Pune, Pimpri-Chinchwad, Maharashtra 411057, India</t>
+          <t>Office no 10, Shrinivas Classic, Baner Rd, above Union Bank of India, near Mauli Garden Mangal Karyala, Shambhu Vihar Society, Baner, Pune, Maharashtra 411069, India</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>+91 20 6791 5400</t>
+          <t>+91 90115 28599</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>https://suryahospitals.com/pune/</t>
+          <t>https://www.drranjeetpatil.com/cardiologist-pune</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>4.4</v>
+        <v>5</v>
       </c>
       <c r="H12" t="n">
-        <v>4902</v>
+        <v>1034</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>A Heartfelt Thank You to Surya Hospital  We recently had the most incredible experience at Surya Hospital, where my wife delivered our beaut | Utterly Disappointed with Surya Hospital Wakad, Pune I had an extremely disappointing and frustrating experience at Surya Hospital Wakad. I  | I would like to provide 5 star rating to Surya hospital. All the doctor and duty staff are really excellent. I always visit this hospital fo | I had a wonderful experience at Surya Hospital. The doctors, nurses, and entire staff were incredibly professional, kind, and supportive thr | Highly recommended! We are truly grateful for the genuine care, treatment, and help provided by Dr. Varshali ma'am.Throughout my wife’s preg</t>
+          <t>—</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>ChIJ0aIl4Fy5wjsRVa3k7WgX9gk</t>
+          <t>ChIJERkflDW_wjsRK_VAbirT7uo</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Wakad, Pune</t>
+          <t>Aundh, Pune</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Dr. Trupti Shekade | Best Child Specialist | Best Paediatrician | Best Neonatologist</t>
+          <t>AIMS Cardiac Hospital | Hospital in Pune | Hospital in Aundh</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Pediatrician</t>
+          <t>Cardiologist</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Dr. Trupti Shekade | Best Child Specialist | Best Paediatrician | Best Neonatologist</t>
+          <t>AIMS Cardiac Hospital | Hospital in Pune | Hospital in Aundh</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>3rd Floor, Little Miracle Children Hospital, WESTWOOD ESTATES, C/O, Hinjawadi Rd, Kaspate Wasti, Wakad, Pune, Pimpri-Chinchwad, Maharashtra 411057, India</t>
+          <t>2nd Floor, AIMS Hospital, Ward No. 8, Aundh Gaon, Aundh, Pune, Maharashtra 411027, India</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>+91 70639 00231</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr"/>
+          <t>+91 92255 39376</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>https://www.cardiologistnearme.co.in/</t>
+        </is>
+      </c>
       <c r="G13" t="n">
-        <v>5</v>
+        <v>4.9</v>
       </c>
       <c r="H13" t="n">
-        <v>34</v>
+        <v>130</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Ethical practice. If you believe in review then I will strongly recommend this hospital. The doctor's are professional and they do take utmo | Congratulations Dr. Trupti on your new facility. I know that you will continue to do well at your new location. Your ability to care for chi | Hospital is very clean &amp; nice. All upgraded machines are available there. Very good, qualified &amp; trustable doctor.  Dr. Trupti Shekde is ver | DR. TRUPTI SHEKDE is an excellent doctor with great knowledge. I recommend her to everyone as she is one of the best pediatrician and this i | One of the best doctor i have come across, always gives personal attention and patiently hears out the problems and gives the best treatment</t>
+          <t>—</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>ChIJ7eBwG3-5wjsRlFgKWm8V-fk</t>
+          <t>ChIJx0g3nDa_wjsRXg5MVnejWUo</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Wakad, Pune</t>
+          <t>Aundh, Pune</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Dr. Sachin Shah</t>
+          <t>Dr Mangesh Danej Heart Clinic and Diagnostics</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Pediatrician</t>
+          <t>Cardiologist</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Dr. Sachin Shah</t>
+          <t>Dr Mangesh Danej Heart Clinic and Diagnostics</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Surya Mother and Child Superspeciality Hospital, Sr no 8 Bhujbal chowk, Near Wakad Octroi Naka and, Hinjawadi Flyover, Bhujbal Vasti, Wakad, Pune, Pimpri-Chinchwad, Maharashtra 411057, India</t>
+          <t>2 nd floor, SHIVOM REGENCY, 202, Baner Rd, above JYOTI GAS APPLIANCES, Baner Gaon, Baner, Pune, Maharashtra 411069, India</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>+91 20 6791 5455</t>
+          <t>+91 73856 26202</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>http://drsachinshah.com/</t>
+          <t>https://puneccclinic.com/</t>
         </is>
       </c>
       <c r="G14" t="n">
         <v>4.9</v>
       </c>
       <c r="H14" t="n">
-        <v>3196</v>
+        <v>439</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Dr. Sachin Shah is truly one of the more experienced and compassionate professionals I’ve come across. His ability to listen patiently and e | We’ve been visiting Dr. Sachin Shah at Surya Hospital ever since our daughter was born here, and I must say – it’s been an incredibly reassu | Dr Sachin Shah is one of the best pediatrician. With his expertise and compassionate attitude he really handles the child issues very effici | We’ve had a fantastic experience with Dr. Sachin Shah. From the very first visit, He made our child feel comfortable, listened carefully to  | As a patient of Dr sachin sir i am very happy to have him.. As my kid is 8 years old and from day 1 he is treating him as his kid. He suppor</t>
+          <t>—</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>ChIJzZP34Fy5wjsRClA94uP8hnU</t>
+          <t>ChIJDaWDR0fBwjsRENZ2y0D0GgA</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Wakad, Pune</t>
+          <t>Aundh, Pune</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>DR.LEENATA'S CHILD CARE CENTRE Children's Clinic Child Hospital Pediatrician</t>
+          <t>The Inamdar Heart Clinic</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Pediatrician</t>
+          <t>Cardiologist</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>DR.LEENATA'S CHILD CARE CENTRE Children's Clinic Child Hospital Pediatrician</t>
+          <t>The Inamdar Heart Clinic</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>opposite Sonigara Landmark, near Pankaj super market, Kaspate Wasti, Wakad, Pune, Pimpri-Chinchwad, Maharashtra 411057, India</t>
+          <t>1st Floor, Hrishikesh Dham(B Lane adjacent to Parihar Sweets, ITI Rd, opposite State Bank of India Parihar Chowk, Sanghvi Nagar, Aundh, Pune, Maharashtra 411067, India</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>+91 72630 89089</t>
+          <t>+91 98220 39863</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>https://technoflybusinesssolutions.com/cards/leenatas-child-care-vaccination-centre-566</t>
+          <t>https://theinamdarheartclinic.com/</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>5</v>
+        <v>4.7</v>
       </c>
       <c r="H15" t="n">
-        <v>105</v>
+        <v>18</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>"One of the finest doctors in Wakad. Good diagnosis and excellent treatment for my son. Very prompt and responsive over the phone. Thank you | We are absolutely grateful to Dr. Leenata for her concept of low/no medicine. Before consulting with her, my 6 month daughter was having 7-8 | Happy parent! My daughter was diagnosed with Dengue. Madam followed all right protocol and made sure the situation is always in control. Tha | Dr. Leenata is a remarkable doctor with extensive knowledge and a compassionate approach, making her a true blessing for our children. She i | "Dr. Leenata is amazing! So caring, knowledgeable, and gentle with patient. Always answers all my questions and puts us at ease. Highly reco</t>
+          <t>—</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>ChIJayMefBa5wjsR-eOD4mxK6BQ</t>
+          <t>ChIJpcngdjC_wjsRAqHT8QnA5C4</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Wakad, Pune</t>
+          <t>Aundh, Pune</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>THE HEART CLINIC By Vivek Manade Cardiologist Pimple Saudagar : Best Cardiologist &amp; Heart Specialist In Pimple Saudagar</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Cardiologist</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>THE HEART CLINIC By Vivek Manade Cardiologist Pimple Saudagar : Best Cardiologist &amp; Heart Specialist In Pimple Saudagar</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>The Heart Clinic, 302 3rd floor, Ganesham Commercial E- Building, near Govind Garden Hotel, Sai Nagar Park, Pimple Saudagar, Pune, Pimpri-Chinchwad, Maharashtra 411027, India</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>+91 85307 97300</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>https://drvivekmanadecardiologist.com/</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>5</v>
+      </c>
+      <c r="H16" t="n">
+        <v>123</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>ChIJi5AtpG-5wjsRxZpJkmqDCP4</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Aundh, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Cardiologist - Sanjivani Medipoint Hospital, Aundh</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Cardiologist</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Cardiologist - Sanjivani Medipoint Hospital, Aundh</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>241/2/1, New DP Rd, Shambhu Vihar Society, Aundh, Pune, Maharashtra 411067, India</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>+91 84848 65633</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>http://www.sanjivanimedipoint.in/</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>5</v>
+      </c>
+      <c r="H17" t="n">
+        <v>20</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>ChIJB7YkCH6_wjsR23dhuSzLf4o</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Aundh, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Pediatrician Dr. Mahesh Sulakshane At Dr.Sulakshane Multi speciality Clinic</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Pediatrician</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Pediatrician Dr. Mahesh Sulakshane At Dr.Sulakshane Multi speciality Clinic</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>201, Dr Sulakshane Multispeciality Clinic, Supreme Square, DP Rd, Raagdari Society, Aundh, Pune, Maharashtra 411067, India</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>+91 20 2588 4157</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/dr.sulakshane/</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="H18" t="n">
+        <v>327</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>ChIJXwAAADu_wjsRddEc3IqyXSE</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Aundh, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Pediatrician Dr Shrinivas Tambe MD FRCPCH(UK) Pediatrician and Neonatologist( Orange Children’s Clinic)</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Pediatrician</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Pediatrician Dr Shrinivas Tambe MD FRCPCH(UK) Pediatrician and Neonatologist( Orange Children’s Clinic)</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>203, Seasons Business Square, Seasons Rd, Sanewadi, Aundh, Pune, Maharashtra 411067, India</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>+91 73991 14400</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>https://www.drshrinivastambe.com/#home</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="H19" t="n">
+        <v>230</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>ChIJQ1VxM9K-wjsR5GzN4YFKrXM</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Aundh, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Pediatrician Dr. Chandrashekhar Phadnis in Aundh</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Pediatrician</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Pediatrician Dr. Chandrashekhar Phadnis in Aundh</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2nd for ajay apartment, above vividha novelties, Sanghvi Nagar, Ward No. 8, Sadhu Vasvani Nagar, Aundh, Pune, Maharashtra 411067, India</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>+91 95792 32565</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>https://avpolyclinics.com/</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>5</v>
+      </c>
+      <c r="H20" t="n">
+        <v>53</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>ChIJFcWY43vBwjsR39BaNq0z2MM</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Aundh, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
           <t>Dr Shridhar Pawale</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B21" t="inlineStr">
         <is>
           <t>Pediatrician</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>Dr Shridhar Pawale</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>Leela Superspeciality Hospital, fourth floor, Westwood Estates Commercial Complex, 403-404, Kaspate Wasti, Wakad, Pune, Pimpri-Chinchwad, Maharashtra 411057, India</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="n">
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="n">
         <v>4.9</v>
       </c>
-      <c r="H16" t="n">
+      <c r="H21" t="n">
         <v>575</v>
       </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>We are so grateful to have found a doctor like him. I don’t know what magic he has he is our baby’s pediatrician from day 1 with just a sing | We are incredibly grateful to have had Dr. Pawale as our baby’s neonatologist and pediatrician. From the very beginning, Dr. Pawale showed n | We have been visiting Dr. Pawale for the last 5 years, and we couldn’t be more grateful. He is truly one of the best! Always patient, caring | Dr. Shridhar Pawale is a very kind and experienced child specialist. From our first visit, I felt confident and comfortable with his approac | He engages with the child very nicely and also with parents to address their concerns. And the best is his proactive personal calling/messag</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
         <is>
           <t>ChIJXRNPIS-5wjsRKtTKbhXMIPk</t>
         </is>
       </c>
-      <c r="K16" t="inlineStr">
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Aundh, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>AV Children Clinic</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Pediatrician</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>AV Children Clinic</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Flat no.6, Ajay Apt, DP road, above Vividha Novelties, near Parihar Chowk, Sanghvi Nagar, Ward No. 8, Sadhu Vasvani Nagar, Aundh, Pune, Maharashtra 411067, India</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>+91 70389 23951</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="n">
+        <v>5</v>
+      </c>
+      <c r="H22" t="n">
+        <v>10</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>ChIJ6er0bDW_wjsRawz9_EWrI9U</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Aundh, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Ankura Hospital for Women &amp; Children - Pune</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Pediatrician</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Ankura Hospital for Women &amp; Children - Pune</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>S.No.163, CTS No.2488, 1+2A+2B/1, Nagras Rd, opposite SBI PBB, Ward No. 8, Wireless Colony, Aundh, Pune, Maharashtra 411067, India</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>+91 90531 08108</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>https://www.ankurahospitals.com/women-and-childcare-hospital-in-pune/</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="H23" t="n">
+        <v>2512</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>ChIJWSbwyhq_wjsRc8IDS864p-Q</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Aundh, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Dr. Umesh Vaidya</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Pediatrician</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Dr. Umesh Vaidya</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Ankura Hospital, Nagras Rd, opposite SBI PBB, Harmony Society, Ward No. 8, Wireless Colony, Aundh, Pune, Maharashtra 411067, India</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>https://www.ankurahospitals.com/doctor/dr-umesh-vaidya/</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="H24" t="n">
+        <v>22</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>ChIJJ7mzUuq_wjsRc0R1sFtjJPg</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Aundh, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Dr. Vidya Nagarajan</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Pediatrician</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Dr. Vidya Nagarajan</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Opp Jai Hind, ITI Rd, near Pariar Chowk, Sanghvi Nagar, Ward No. 8, Sadhu Vasvani Nagar, Aundh, Pune, Maharashtra 411007, India</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>+91 94220 09704</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H25" t="n">
+        <v>31</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>ChIJk862gTq_wjsRpyaPvQ9ErRY</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Aundh, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>SkinEthics</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Dermatologist</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>SkinEthics</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Office no.3, 2nd floor, Windsor Commerce, Baner Rd, near Wadeshwar Hotel, Baner, Pune, Maharashtra 411069, India</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>+91 90282 91234</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>https://skinethicspune.com/</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="H26" t="n">
+        <v>637</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>ChIJRaf6ati-wjsRuCFazZb3EdA</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Baner, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Allure Clinic</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Dermatologist</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Allure Clinic</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Office number 4,5 and 6, Kapil Classic, Baner Rd, above bank of Maharashtra, Baner Bio-Diversity Park, Baner, Pune, Maharashtra 411069, India</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>+91 72765 74567</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>https://allureclinic.in/</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="H27" t="n">
+        <v>619</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>ChIJ1_9sMNi-wjsR-qeQDyvfTWE</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Baner, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Skin 101 | Dr. Tanvi Komawar Adgudwar | Best Skin Specialist in Baner | Aesthetic clinic in Baner</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Dermatologist</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Skin 101 | Dr. Tanvi Komawar Adgudwar | Best Skin Specialist in Baner | Aesthetic clinic in Baner</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2nd floor Whispering woods building, Ganraj chowk, opposite Gera emerald city, Veerbhadra Nagar, Baner, Pune, Maharashtra 411069, India</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>+91 70551 01101</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>http://www.the101clinic.com/</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="H28" t="n">
+        <v>232</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>ChIJrSw-5_W_wjsRm54QzgQVpEA</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>Baner, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Clear Skin Clinic Baner</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Dermatologist</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Clear Skin Clinic Baner</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Vasukamal Survey No. 85/2A/4, Office No 301 302, Ganraj Mangal Karyalay Chowk, Lalit Estate, Baner, Pune, Maharashtra 411069, India</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>+91 95845 84111</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>https://www.clearskin.in/best-skin-care-clinic-baner-pune/</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="H29" t="n">
+        <v>304</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>ChIJse3Y9s-_wjsRBpuyjnPbUyo</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>Baner, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Viva Luxe by Dr. Sonnal Chavaan | Dermatologist In Pune, Baner | Skin Specialist in Pune</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Dermatologist</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Viva Luxe by Dr. Sonnal Chavaan | Dermatologist In Pune, Baner | Skin Specialist in Pune</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>302, Royal Fortune, Pan Card Club Rd, next to Supreme Amadore, Baner, Pune, Maharashtra 411045, India</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>+91 91750 06629</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>https://skinspecialistnearme.co.in/</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="H30" t="n">
+        <v>261</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>ChIJ08xZ4EG_wjsRrcaoaXrCY2o</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>Baner, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Radiant Skin &amp; Hair Clinic</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Dermatologist</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Radiant Skin &amp; Hair Clinic</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>K Square, Office No.308, 3rd Floor Shroff Marg, Pan Card Club Rd, near Union Bank, Baner, Pune, Maharashtra 411069, India</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>+91 98224 96166</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>https://radiantskinandhair.in/</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="H31" t="n">
+        <v>458</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>ChIJPZZXK9i-wjsRYgcT0w6_p6s</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>Baner, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Neo Plant Advance Hair and Skin Clinic</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Dermatologist</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Neo Plant Advance Hair and Skin Clinic</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Office Number- 306, Altus, Building Name -Altus, next to Tatva Restaurant, Laxman Nagar, Baner, Pune, Maharashtra 411045, India</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>+91 84339 20504</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>https://neoplanthairclinic.com/</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>5</v>
+      </c>
+      <c r="H32" t="n">
+        <v>410</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>ChIJ39Kb5UW5wjsR2D45T6XaNoM</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>Baner, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Dr. Devayani Pol's Tejomed Skin &amp; Aesthetic Clinic - Best Dermatologist in Baner, Pune</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Dermatologist</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Dr. Devayani Pol's Tejomed Skin &amp; Aesthetic Clinic - Best Dermatologist in Baner, Pune</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>OPD 1, 506, 66highstreet square, Pan Card Club Rd, Baner Gaon, Baner, Pune, Maharashtra 411069, India</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>https://tejomed.in/</t>
+        </is>
+      </c>
+      <c r="G33" t="n">
+        <v>5</v>
+      </c>
+      <c r="H33" t="n">
+        <v>37</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>ChIJGy8o0g2_wjsR7qKnlZrk6_E</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>Baner, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Dr. Kartik Bhosale Cardiology Clinic | DM-Cardiologist, Heart Specialist, 2D Echo, Angiography, Stress Test/TMT in Baner Pune</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Cardiologist</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Dr. Kartik Bhosale Cardiology Clinic | DM-Cardiologist, Heart Specialist, 2D Echo, Angiography, Stress Test/TMT in Baner Pune</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Shop no. 2, Vedant Healthcare Clinic, KALAMKAR COMPLEX, Balewadi Phata, Baner, Pune, Maharashtra 411069, India</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>+91 92721 10071</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>https://www.drbhosalekartik.com/best-cardiologist-in-baner/</t>
+        </is>
+      </c>
+      <c r="G34" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="H34" t="n">
+        <v>44</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>ChIJETGFQWW_wjsRXE_3biZ5JK8</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>Baner, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Dr. Abhijit Joshi | Best Cardiologist in Baner</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Cardiologist</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Dr. Abhijit Joshi | Best Cardiologist in Baner</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Room No. 16, Manipal Hospital Survey No 111/11/1, Veerbhadra Nagar Rd, opposite D-MART, Veerbhadra Nagar, Baner, Pune, Maharashtra 411069, India</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>+91 20 6813 8844</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>https://www.manipalhospitals.com/baner/doctors/dr-abhijit-joshi-cardiologist/</t>
+        </is>
+      </c>
+      <c r="G35" t="n">
+        <v>5</v>
+      </c>
+      <c r="H35" t="n">
+        <v>32</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>ChIJRz4Y40G_wjsRViD_kKShCdI</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>Baner, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Dr Abhay Khode-Best Cardiologist in Baner | Heart Specialist,Cardiology Doctor,Cardiologist in Baner,Balewadi,Aundh,Pune</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Cardiologist</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Dr Abhay Khode-Best Cardiologist in Baner | Heart Specialist,Cardiology Doctor,Cardiologist in Baner,Balewadi,Aundh,Pune</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>B103,B.U.Bhandari Hillside,Phase1, Baner Rd, near Cafe Coffee Day, Baner Bio-Diversity Park, Baner, Pune, Maharashtra 411069, India</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>+91 80 4803 4071</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>http://www.drkhodecardiovision.com/</t>
+        </is>
+      </c>
+      <c r="G36" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="H36" t="n">
+        <v>41</v>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>ChIJcXST_-i_wjsRlIgZ1vwTngk</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>Baner, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Dr. Pranav Deshmukh Shende's TejoMed Heart Clinic- Best Cardiologist in Baner</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Cardiologist</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Dr. Pranav Deshmukh Shende's TejoMed Heart Clinic- Best Cardiologist in Baner</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>OPD no 2, 5th Floor 506, 66highstreet square, Pan Card Club Rd, Baner, Pune, Maharashtra 411069, India</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr"/>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>https://tejomed.in/dr-pranav-deshmukh/</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
+        <v>5</v>
+      </c>
+      <c r="H37" t="n">
+        <v>22</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>ChIJPbJ24a2_wjsR3x-lHqzLk0M</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>Baner, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Dr.Kadam Heart Clinic &amp; diagnostic centre</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Cardiologist</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Dr.Kadam Heart Clinic &amp; diagnostic centre</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Dr. Kadam heart clinic, Plot no.36, Sahil Serene Road, off Pan Card Club Road, opposite Sai Vatika, Shivneri Colony, Samarth Colony, Baner, Pune, Maharashtra 411069, India</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>+91 94201 96691</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="H38" t="n">
+        <v>381</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>ChIJhV5n5lW_wjsRs10A9ngZjqQ</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>Baner, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Dr Yuvaraj Bhosale</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Cardiologist</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Dr Yuvaraj Bhosale</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Sumitz ,1st floor, Krishna Avenue, Baner Rd, opp. D-mart, above Domino's, Veerbhadra Nagar, Baner, Pune, Maharashtra 411069, India</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>+91 84229 84545</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="n">
+        <v>5</v>
+      </c>
+      <c r="H39" t="n">
+        <v>61</v>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>ChIJAaloFV6_wjsRGV9T9ogqjzk</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>Baner, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Dr. Ashwini's Kidz Clinic and Child Vaccination Centre | Pediatrician in Baner | Child Specialist | Children Clinic In Baner</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Pediatrician</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Dr. Ashwini's Kidz Clinic and Child Vaccination Centre | Pediatrician in Baner | Child Specialist | Children Clinic In Baner</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>2nd Floor, Shiv Datta Complex, above Lifecare medical store, near Orchid school, Balewadi Phata, Baner, Pune, Maharashtra 411069, India</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>+91 86689 72250</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>https://www.practo.com/pune/doctor/dr-ashwini-karale-patil-pediatrician</t>
+        </is>
+      </c>
+      <c r="G40" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="H40" t="n">
+        <v>89</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>ChIJiRvd9OK_wjsRi76SEI06gfU</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>Baner, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Umarji Mother and Child Care Hospital (उमरजी माता आणि लहान मुलांचे रुग्णालय)</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Pediatrician</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Umarji Mother and Child Care Hospital (उमरजी माता आणि लहान मुलांचे रुग्णालय)</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Survey no. 13/1, Umarji Mother and Child Care hospital, beside Aditya Shagun "Comfort zone, Balewadi Phata, Baner, Pune, Maharashtra 411045, India</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>+91 20 3503 2200</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>https://umarjihealthcare.com/</t>
+        </is>
+      </c>
+      <c r="G41" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="H41" t="n">
+        <v>3529</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>ChIJ6RkI7DK5wjsR5_U7MDh5N_I</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>Baner, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Dr. Meera Singhal</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Pediatrician</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Dr. Meera Singhal</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Prachi Residency, 1, Baner Rd, opp. KAPIL MALHAR, Society, Baner, Pune, Maharashtra 411069, India</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>+91 98600 90250</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="H42" t="n">
+        <v>51</v>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>ChIJr4pjpdG-wjsRDsfgI4a2muU</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>Baner, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Dr. Dhekne Clinic</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Pediatrician</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Dr. Dhekne Clinic</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Office 2B, The Fountainhead, Baner - Balewadi Rd, Balewadi Phata, Baner, Pune, Maharashtra 411069, India</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>+91 97637 23378</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="H43" t="n">
+        <v>225</v>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>ChIJwXrnTM2-wjsR9FIAlpk8IA8</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>Baner, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Dr. Babita Nawalkar - Children clinic in Baner, Best Pediatrician in Baner</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Pediatrician</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Dr. Babita Nawalkar - Children clinic in Baner, Best Pediatrician in Baner</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>First floor, Narayani building, Pan Card Club Rd, near Kapil Akhila, Baner Gaon, Baner, Pune, Maharashtra 411069, India</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>+91 86056 77836</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>https://www.drbabitanawalkar.com/</t>
+        </is>
+      </c>
+      <c r="G44" t="n">
+        <v>5</v>
+      </c>
+      <c r="H44" t="n">
+        <v>8</v>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>ChIJ20cBB3u_wjsR9ayTuuuPqmo</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>Baner, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Dr. Ujjwala Keskar | Best Pediatrics &amp; Child Care in Baner</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Pediatrician</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Dr. Ujjwala Keskar | Best Pediatrics &amp; Child Care in Baner</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Room No. 29, Manipal Hospital, Survey No 111, 11/1, Mhalunge Main Road, opposite D-MART, Veerbhadra Nagar, Baner, Pune, Maharashtra 411069, India</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>+91 20 6813 8844</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>https://www.manipalhospitals.com/baner/doctors/dr-ujjwalla-keskar/</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="H45" t="n">
+        <v>6</v>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>ChIJ1dem-4e_wjsRYKDa7rbWiEI</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>Baner, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Dr Avinash Bhore</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Pediatrician</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Dr Avinash Bhore</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Office no 1, Sr.no.78, Kalamkar Paradise, 3/4, Balewadi Phata, Baner, Pune, Maharashtra 411069, India</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>+91 98904 11957</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="H46" t="n">
+        <v>47</v>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>ChIJZ5aW_9G-wjsRaxYwIJ7LbkY</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>Baner, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>EVA PIMPLES SKIN &amp; HAIR CLINIC</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Dermatologist</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>EVA PIMPLES SKIN &amp; HAIR CLINIC</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Flat no 201, Second floor, Aabai Tower, Mauli Chowk, Datta Mandir Rd, Shankar Kalat Nagar, Wakad, Pune, Pimpri-Chinchwad, Maharashtra 411057, India</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>+91 788 799 1919</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>https://evaskinclinicpune.com/?utm_source=google&amp;utm_medium=GMB&amp;utm_campaign=GMB+Clicks&amp;utm_id=123&amp;utm_term=GMB+&amp;utm_content=GMB+</t>
+        </is>
+      </c>
+      <c r="G47" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="H47" t="n">
+        <v>1353</v>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>ChIJR35CyOe5wjsRY4MZr6SI5tE</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>Wakad, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Dr. Kiran Ardad Mane - Best Dermatologist &amp; Cosmetologist in PCMC, Pune | Skin &amp; Hair Specialist in Wakad | Leela Hospital</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Dermatologist</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Dr. Kiran Ardad Mane - Best Dermatologist &amp; Cosmetologist in PCMC, Pune | Skin &amp; Hair Specialist in Wakad | Leela Hospital</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Leela Super- speciality Hospital FOURTH FLOOR, Office 403, Westwood Estates Commercial Complex, 404, Mont Vert Tropez Rd, near Mhatoba chowk, Kaspate Wasti, Wakad, Pimpri-Chinchwad, Maharashtra 411057, India</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>+91 93223 00500</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>https://www.leelasuperspecialityhospital.com/dr-kiran-ardad-mane/</t>
+        </is>
+      </c>
+      <c r="G48" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="H48" t="n">
+        <v>409</v>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>ChIJ4aPaJn65wjsRnjd15ocXguY</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>Wakad, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Dr. Mamta Patil - The Skin N Hair Clinic</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Dermatologist</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Dr. Mamta Patil - The Skin N Hair Clinic</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>111, 1st Floor, Sonigara Landmark, near PNB Bank, Dynasty Society, Kaspate Wasti, Wakad, Pune, Pimpri-Chinchwad, Maharashtra 411054, India</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>+91 70667 91791</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>https://www.drmamtapatil.in/</t>
+        </is>
+      </c>
+      <c r="G49" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="H49" t="n">
+        <v>359</v>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>ChIJ2d4qZKi5wjsRSLlaiZK6BXE</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>Wakad, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>The Skin Doctors - Skin Hair &amp; Laser Centre in Pimple Saudagar</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Dermatologist</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>The Skin Doctors - Skin Hair &amp; Laser Centre in Pimple Saudagar</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Shop 126-127, Vision 9 Mall, Kunal Icon Rd, Pimple Saudagar, Pimpri-Chinchwad, Maharashtra 411027, India</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>+91 93736 57799</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>https://www.theskindoctors.in/pimplesaudagar</t>
+        </is>
+      </c>
+      <c r="G50" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="H50" t="n">
+        <v>1294</v>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>ChIJbRN91R65wjsR4ToCmKitISE</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>Wakad, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>The Skin Doctors - Skin Clinic | Dermatologist | Hair Doctor</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Dermatologist</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>The Skin Doctors - Skin Clinic | Dermatologist | Hair Doctor</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Rama Equator, Complex, Ajmera Main Rd, Morewadi, Pimpri Colony, Pimpri-Chinchwad, Maharashtra 411018, India</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>+91 93735 57766</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>http://theskindoctors.in/?utm_source=google&amp;utm_medium=wix_google_business_profile&amp;utm_campaign=17353780241968726606</t>
+        </is>
+      </c>
+      <c r="G51" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="H51" t="n">
+        <v>1906</v>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>ChIJAQAAAES4wjsRPdcO2iiE_ZA</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>Wakad, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Dr. Madhavi's Skin Central Skin &amp; Hair Clinic| Dermatologist in Wakad, Pune</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Dermatologist</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Dr. Madhavi's Skin Central Skin &amp; Hair Clinic| Dermatologist in Wakad, Pune</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Shop No, Gr Flr, Sanskriti Arcade, 7 &amp; 8, opposite PCMC school, Kaspate Wasti, Wakad, Pune, Pimpri-Chinchwad, Maharashtra 411057, India</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>+91 70204 56767</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>https://theskincentral.com/</t>
+        </is>
+      </c>
+      <c r="G52" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="H52" t="n">
+        <v>172</v>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>ChIJJQAAwD-5wjsR7JcdaO5xZ5w</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>Wakad, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Skin Elite Clinic | Skin and Hair clinic in Wakad | Best Skin and Hair specialist Clinic / Best Skin specialist in wakad</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Dermatologist</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Skin Elite Clinic | Skin and Hair clinic in Wakad | Best Skin and Hair specialist Clinic / Best Skin specialist in wakad</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Shop No 5, Above Medicine point medical, Prudentia Tower, Mauli Chowk, Datta Mandir Rd, Shankar Kalat Nagar, Wakad, Pune, Pimpri-Chinchwad, Maharashtra 411057, India</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>+91 70570 37225</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>https://www.skineliteclinics.com/</t>
+        </is>
+      </c>
+      <c r="G53" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="H53" t="n">
+        <v>152</v>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>ChIJEanaNxe5wjsRq-0ZqwJB6NA</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>Wakad, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Dr. Manisha Shirbhate's Arnav Skin and Hair clinic</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Dermatologist</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Dr. Manisha Shirbhate's Arnav Skin and Hair clinic</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Echoing Green, office 203, Shankar Kalate Nagar Rd, near Eden Garden, Shankar Kalat Nagar, Wakad, Pune, Pimpri-Chinchwad, Maharashtra 411057, India</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>+91 86052 73370</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr"/>
+      <c r="G54" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="H54" t="n">
+        <v>128</v>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>ChIJKxlH_Pe5wjsRKu0CtKUWW5w</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>Wakad, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Dr. Kartik Bhosale Cardiology Clinic | DM-Cardiologist, Heart Specialist, 2D Echo, Angiography, Stress Test/TMT in Wakad Pune</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Cardiologist</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Dr. Kartik Bhosale Cardiology Clinic | DM-Cardiologist, Heart Specialist, 2D Echo, Angiography, Stress Test/TMT in Wakad Pune</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Office No 207, Second floor, Dr Kartik Bhosale’s Cardiology Clinic, Oriana Crest building, Datta Mandir Rd, Postal Colony, Shankar Kalat Nagar, Wakad, Pune, Pimpri-Chinchwad, Maharashtra 411057, India</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>+91 84200 70081</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>https://www.drbhosalekartik.com/</t>
+        </is>
+      </c>
+      <c r="G55" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="H55" t="n">
+        <v>821</v>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>ChIJHS4DsoK5wjsR951ft9pm4lY</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>Wakad, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Dr Ajit Jadhav MD DNB Cardiologist in Pimple Saudagar |ECG, 2D Echo , TMT</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Cardiologist</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Dr Ajit Jadhav MD DNB Cardiologist in Pimple Saudagar |ECG, 2D Echo , TMT</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Shop 1C, 1st floor, Kunjir Shyama Prestige, near, Kokane Chowk, above Just Casuals, opposite विजय सेल्स, Pimple Saudagar, Pune, Pimpri-Chinchwad, Maharashtra 411027, India</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>+91 90288 98494</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>http://www.drjadhavclinic.com/</t>
+        </is>
+      </c>
+      <c r="G56" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="H56" t="n">
+        <v>368</v>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>ChIJMRmVXry5wjsRZFMW6xQqbFQ</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>Wakad, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Dr. Thopte's Heart Care Clinic Wakad | Heart Specialist| 2D Echo | ECG |Angiography | TMT| Cardiologist In Wakad| Pune</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Cardiologist</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Dr. Thopte's Heart Care Clinic Wakad | Heart Specialist| 2D Echo | ECG |Angiography | TMT| Cardiologist In Wakad| Pune</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Shop no. 1A, WINDWARDS SOCIETY, E - Wing, Chatrapati Chowk Rd, Kaspate Wasti, Wakad, Pimpri-Chinchwad, Pune, Maharashtra 411057, India</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>+91 90113 33339</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="H57" t="n">
+        <v>58</v>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>ChIJ7Q997q-5wjsRPuBG_ZVrjg8</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>Wakad, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Dr Mahesh Kharade</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Cardiologist</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Dr Mahesh Kharade</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>****ABOVE FEDARAL BANK***, Saarathi Superspeciality Clinic, Shri Ganesh Imperia, Datta Mandir Rd, Shankar Kalat Nagar, Wakad, Pune, Pimpri-Chinchwad, Maharashtra 411057, India</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>+91 83292 79367</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>https://www.saarathihealthcare.in/</t>
+        </is>
+      </c>
+      <c r="G58" t="n">
+        <v>5</v>
+      </c>
+      <c r="H58" t="n">
+        <v>40</v>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>ChIJ2VQrqn65wjsRQi2DwOmYFTQ</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>Wakad, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Dr Sachin Hundekari Elite heart and diabetic clinic | Pathology Lab | Cardiologist in Wakad</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Cardiologist</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Dr Sachin Hundekari Elite heart and diabetic clinic | Pathology Lab | Cardiologist in Wakad</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Elite Heart Clinic, Shop No. 209, Solitaire Business Hub Road, Kalewadi Phata, Kaspate Wasti, Wakad, Pune, Pimpri-Chinchwad, Maharashtra 411057, India</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>+91 80074 17756</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr"/>
+      <c r="G59" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="H59" t="n">
+        <v>589</v>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>ChIJN9mGSxK5wjsRjfz4dtQnnzU</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>Wakad, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Dr.Pranay Jambhulkar’s Karunya Heart Clinic |Best Cardiologist in Pune |MD ,DM Cardiology |2D ECHO| TMT|Diabetologist</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Cardiologist</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Dr.Pranay Jambhulkar’s Karunya Heart Clinic |Best Cardiologist in Pune |MD ,DM Cardiology |2D ECHO| TMT|Diabetologist</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>First Floor, Shop No. 110, Wbiz Commercial complex, Bhumkar Chowk Rd, Wakad, Pimpri-Chinchwad, Pune, Maharashtra 411057, India</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>+91 94239 37304</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>http://karunyaheartclinic.com/</t>
+        </is>
+      </c>
+      <c r="G60" t="n">
+        <v>5</v>
+      </c>
+      <c r="H60" t="n">
+        <v>108</v>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>ChIJBXTU4ju5wjsR1zlVCR9TvpA</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>Wakad, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Dr. Hundekari's Elite Heart and Diabetic Clinic | Pathology Lab | Cardiologist in Wakad</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Cardiologist</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Dr. Hundekari's Elite Heart and Diabetic Clinic | Pathology Lab | Cardiologist in Wakad</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>JQ2G+C5H, Vishnu Dev Nagar, Wakad, Pimpri-Chinchwad, Maharashtra 411057, India</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>+91 80074 17756</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>https://eliteheartclinic.com/</t>
+        </is>
+      </c>
+      <c r="G61" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="H61" t="n">
+        <v>87</v>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>ChIJUePLSBK5wjsRke-ruOvrsJA</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>Wakad, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Wellness Edge Clinic Best Cardiologist &amp; Heart Specialist in Nigdi (Pimpri Chinchwad)</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Cardiologist</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Wellness Edge Clinic Best Cardiologist &amp; Heart Specialist in Nigdi (Pimpri Chinchwad)</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>135, First Floor, Thermax Chowk, KOHINOOR MAJESTIC, behind Kundan Hundai Showroom, Premsadan Housing Society, Ajantha Nagar, Chinchwad, Pune, Pimpri-Chinchwad, Maharashtra 411019, India</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>+91 76662 38079</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr"/>
+      <c r="G62" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="H62" t="n">
+        <v>611</v>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>ChIJH2J8_gq5wjsRmcTAdLftPdA</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>Wakad, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Dr. Sachin Shah</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Pediatrician</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Dr. Sachin Shah</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Surya Mother and Child Superspeciality Hospital, Sr no 8 Bhujbal chowk, Near Wakad Octroi Naka and, Hinjawadi Flyover, Bhujbal Vasti, Wakad, Pune, Pimpri-Chinchwad, Maharashtra 411057, India</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>+91 20 6791 5455</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>http://drsachinshah.com/</t>
+        </is>
+      </c>
+      <c r="G63" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="H63" t="n">
+        <v>3196</v>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>ChIJzZP34Fy5wjsRClA94uP8hnU</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>Wakad, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>DR.LEENATA'S CHILD CARE CENTRE Children's Clinic Child Hospital Pediatrician</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Pediatrician</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>DR.LEENATA'S CHILD CARE CENTRE Children's Clinic Child Hospital Pediatrician</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>opposite Sonigara Landmark, near Pankaj super market, Kaspate Wasti, Wakad, Pune, Pimpri-Chinchwad, Maharashtra 411057, India</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>+91 72630 89089</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>https://technoflybusinesssolutions.com/cards/leenatas-child-care-vaccination-centre-566</t>
+        </is>
+      </c>
+      <c r="G64" t="n">
+        <v>5</v>
+      </c>
+      <c r="H64" t="n">
+        <v>105</v>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>ChIJayMefBa5wjsR-eOD4mxK6BQ</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>Wakad, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Surya Mother And Child Super Speciality Hospital, Hinjewadi</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Pediatrician</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Surya Mother And Child Super Speciality Hospital, Hinjewadi</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Pune Octroi Naka, Sr. No. 8 near Bhujbal Chowk Mumbai Hwy Hinjawadi, Wakad Rd, Bhujbal Vasti, Wakad, Pune, Pimpri-Chinchwad, Maharashtra 411057, India</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>+91 20 6791 5400</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>https://suryahospitals.com/pune/</t>
+        </is>
+      </c>
+      <c r="G65" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="H65" t="n">
+        <v>4902</v>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>ChIJ0aIl4Fy5wjsRVa3k7WgX9gk</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>Wakad, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Dr. Trupti Shekade | Best Child Specialist | Best Paediatrician | Best Neonatologist</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Pediatrician</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Dr. Trupti Shekade | Best Child Specialist | Best Paediatrician | Best Neonatologist</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>3rd Floor, Little Miracle Children Hospital, WESTWOOD ESTATES, C/O, Hinjawadi Rd, Kaspate Wasti, Wakad, Pune, Pimpri-Chinchwad, Maharashtra 411057, India</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>+91 70639 00231</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr"/>
+      <c r="G66" t="n">
+        <v>5</v>
+      </c>
+      <c r="H66" t="n">
+        <v>34</v>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>ChIJ7eBwG3-5wjsRlFgKWm8V-fk</t>
+        </is>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>Wakad, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Dr. Mustapure's Child Clinic</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Pediatrician</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Dr. Mustapure's Child Clinic</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>2nd floor, Grand Heritage, Kaspate Wasti Rd, opposite Ambience hotel, Vishnu Dev Nagar, Wakad, Pimpri-Chinchwad, Maharashtra 411057, India</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>+91 70831 40369</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr"/>
+      <c r="G67" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="H67" t="n">
+        <v>386</v>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>ChIJrU0gQe-7wjsRXDfgDEtaBIs</t>
+        </is>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>Wakad, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Dr.Kapil Jadhav</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Pediatrician</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Dr.Kapil Jadhav</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Clinic No.1/2, Dr. Mande's Clinic, VARDHAMAN PLAZA, opp. Dynasty Society Road, near Radha Pure Veg, Kaspate Wasti, Wakad, Pune, Pimpri-Chinchwad, Maharashtra 411057, India</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr"/>
+      <c r="F68" t="inlineStr"/>
+      <c r="G68" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="H68" t="n">
+        <v>192</v>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>ChIJtSsVsRO5wjsRvFpxurCZT60</t>
+        </is>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>Wakad, Pune</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Dr. Nikhil Patil - Pediatrician, Child Clinic, Child Doctor, Child Specialist in Hinjewadi, Pediatrician in Wakad</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Pediatrician</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Dr. Nikhil Patil - Pediatrician, Child Clinic, Child Doctor, Child Specialist in Hinjewadi, Pediatrician in Wakad</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>2nd Floor, Swasti Clinic, Ram Height, near D' Mart, above Bata Showroom, Hinjawadi, Pune, Pimpri-Chinchwad, Maharashtra 411057, India</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>+91 72492 98207</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>https://swasticlinicpune.in/</t>
+        </is>
+      </c>
+      <c r="G69" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="H69" t="n">
+        <v>234</v>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>ChIJUZwykXq7wjsRlJZEPoLlGmA</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr">
         <is>
           <t>Wakad, Pune</t>
         </is>

</xml_diff>